<commit_message>
Add Tool Management System.
</commit_message>
<xml_diff>
--- a/Flow Chart/Percent.xlsx
+++ b/Flow Chart/Percent.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F2D92E-A66E-4062-917A-C1F15789FFFC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C66A66-F6AD-4A84-977D-FBE9547100CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,7 +156,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]mmmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\-yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -224,22 +224,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,47 +536,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
     </row>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="3">
         <v>43313</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>43344</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>43374</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>43405</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>43435</v>
       </c>
     </row>
@@ -587,15 +587,15 @@
       <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
@@ -604,17 +604,17 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
@@ -623,17 +623,17 @@
       <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
@@ -642,19 +642,19 @@
       <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
@@ -663,11 +663,11 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
@@ -676,11 +676,11 @@
       <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
@@ -689,11 +689,11 @@
       <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="7"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
@@ -702,11 +702,11 @@
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="7"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
@@ -715,11 +715,11 @@
       <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="7"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
@@ -728,11 +728,11 @@
       <c r="D13" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
@@ -741,11 +741,11 @@
       <c r="D14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="7"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
@@ -754,11 +754,11 @@
       <c r="D15" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
@@ -767,11 +767,11 @@
       <c r="D16" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
@@ -780,11 +780,11 @@
       <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
@@ -793,11 +793,11 @@
       <c r="D18" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
@@ -806,11 +806,11 @@
       <c r="D19" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
@@ -819,11 +819,11 @@
       <c r="D20" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
@@ -832,11 +832,11 @@
       <c r="D21" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
@@ -845,11 +845,11 @@
       <c r="D22" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
@@ -858,54 +858,54 @@
       <c r="D23" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
     </row>
     <row r="28" spans="3:9" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="3"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="2"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="4">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="3">
         <v>43313</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="3">
         <v>43344</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>43374</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="3">
         <v>43405</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="3">
         <v>43435</v>
       </c>
     </row>
@@ -916,11 +916,11 @@
       <c r="D31" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
@@ -929,15 +929,15 @@
       <c r="D32" t="s">
         <v>4</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
@@ -946,11 +946,11 @@
       <c r="D33" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
@@ -959,19 +959,19 @@
       <c r="D34" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F34" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G34" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H34" s="9" t="s">
+      <c r="H34" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I34" s="7"/>
+      <c r="I34" s="6"/>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
@@ -980,11 +980,11 @@
       <c r="D35" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="7"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="6"/>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
@@ -993,11 +993,11 @@
       <c r="D36" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
@@ -1006,11 +1006,11 @@
       <c r="D37" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="7"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="6"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
@@ -1019,11 +1019,11 @@
       <c r="D38" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="7"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="6"/>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
@@ -1032,11 +1032,11 @@
       <c r="D39" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="7"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="6"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
@@ -1045,11 +1045,11 @@
       <c r="D40" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="7"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="6"/>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
@@ -1058,11 +1058,11 @@
       <c r="D41" t="s">
         <v>11</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="7"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="6"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
@@ -1071,11 +1071,11 @@
       <c r="D42" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
@@ -1084,11 +1084,11 @@
       <c r="D43" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="6"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
@@ -1097,11 +1097,11 @@
       <c r="D44" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="6"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
@@ -1110,11 +1110,11 @@
       <c r="D45" t="s">
         <v>29</v>
       </c>
-      <c r="E45" s="6"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
     </row>
     <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
@@ -1123,11 +1123,11 @@
       <c r="D46" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="6"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
     </row>
     <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
@@ -1136,11 +1136,11 @@
       <c r="D47" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="6"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
@@ -1149,11 +1149,11 @@
       <c r="D48" t="s">
         <v>32</v>
       </c>
-      <c r="E48" s="6"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
@@ -1162,11 +1162,11 @@
       <c r="D49" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="6"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
@@ -1175,22 +1175,22 @@
       <c r="D50" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="6"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:H29"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:H29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>